<commit_message>
Adding boss cards and chits, revisions after first play test
</commit_message>
<xml_diff>
--- a/data/BossFight.xlsx
+++ b/data/BossFight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adsil\Squib\boss-fight\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E252696A-8353-4D6F-A955-A5507490DD5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFC18D2-F8AE-452B-9F1A-E2F4FBB594EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="336" windowWidth="17280" windowHeight="11244" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2676" yWindow="648" windowWidth="17280" windowHeight="11244" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Equipment" sheetId="4" r:id="rId4"/>
     <sheet name="BossActions" sheetId="6" r:id="rId5"/>
     <sheet name="Bosses" sheetId="5" r:id="rId6"/>
+    <sheet name="Chits" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="286">
   <si>
     <t>Level</t>
   </si>
@@ -212,9 +213,6 @@
     <t>Heal 2</t>
   </si>
   <si>
-    <t>Heal 1 + [int]</t>
-  </si>
-  <si>
     <t>Foresee</t>
   </si>
   <si>
@@ -239,9 +237,6 @@
     <t>Energize</t>
   </si>
   <si>
-    <t>Draw a card.</t>
-  </si>
-  <si>
     <t>Energize 2</t>
   </si>
   <si>
@@ -338,9 +333,6 @@
     <t>Spikes</t>
   </si>
   <si>
-    <t>Empty</t>
-  </si>
-  <si>
     <t>Web</t>
   </si>
   <si>
@@ -380,48 +372,24 @@
     <t>Short Sword</t>
   </si>
   <si>
-    <t>Hand</t>
-  </si>
-  <si>
     <t>[ap] [ap]</t>
   </si>
   <si>
-    <t>cross1.png</t>
-  </si>
-  <si>
-    <t>Deal 2 + [str] damage to creature.</t>
-  </si>
-  <si>
     <t>Broad Sword</t>
   </si>
   <si>
     <t>[ap] [ap] [ap]</t>
   </si>
   <si>
-    <t>Deal 3 + [str] damage to creature.</t>
-  </si>
-  <si>
     <t>War Axe</t>
   </si>
   <si>
-    <t>Deal 4 + [str] damage to creature.</t>
-  </si>
-  <si>
     <t>Bow</t>
   </si>
   <si>
     <t>[ap] [ar]</t>
   </si>
   <si>
-    <t>cross3.png</t>
-  </si>
-  <si>
-    <t>Deal [agl] damage to creature.</t>
-  </si>
-  <si>
-    <t>Bow of Confusion</t>
-  </si>
-  <si>
     <t>[ap] [ar] [po]</t>
   </si>
   <si>
@@ -443,93 +411,42 @@
     <t>[ap] [po]</t>
   </si>
   <si>
-    <t>Deal [agl] damage to creature. If that attack hits, inflict poison 2.</t>
-  </si>
-  <si>
     <t>Fireball</t>
   </si>
   <si>
-    <t>Spell</t>
-  </si>
-  <si>
     <t>[ap] [fi] [fi] [fi]</t>
   </si>
   <si>
-    <t>square2.png</t>
-  </si>
-  <si>
-    <t>Deal 6 + [int] damage to creature.</t>
-  </si>
-  <si>
     <t>Fireball 2</t>
   </si>
   <si>
     <t>[ap] [fi] [fi] [fi] [fi]</t>
   </si>
   <si>
-    <t>Deal 8 + [int] damage to creature.</t>
-  </si>
-  <si>
     <t>Ice Shard</t>
   </si>
   <si>
     <t>[ap] [wa] [wa] [wa]</t>
   </si>
   <si>
-    <t>Deal 5 + [int] damage to creature. That creature can't move this round.</t>
-  </si>
-  <si>
     <t>Poison Spell</t>
   </si>
   <si>
     <t>[ap] [po] [po] [po]</t>
   </si>
   <si>
-    <t xml:space="preserve">Deal 5 damage to creature. Shuffle [int] poison cards into its action deck. </t>
-  </si>
-  <si>
     <t>HP</t>
   </si>
   <si>
     <t>APT</t>
   </si>
   <si>
-    <t>@Agility</t>
-  </si>
-  <si>
-    <t>Agility</t>
-  </si>
-  <si>
-    <t>@Strength</t>
-  </si>
-  <si>
-    <t>Strength</t>
-  </si>
-  <si>
-    <t>@Intelligence</t>
-  </si>
-  <si>
-    <t>Intelligence</t>
-  </si>
-  <si>
     <t>Movement</t>
   </si>
   <si>
     <t>Flavor</t>
   </si>
   <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Deals 4 damage.</t>
-  </si>
-  <si>
-    <t>Deals 6 damage.</t>
-  </si>
-  <si>
-    <t>Deals 2 damage.</t>
-  </si>
-  <si>
     <t>Heal for 3.</t>
   </si>
   <si>
@@ -659,15 +576,9 @@
     <t>1 damage when entering.</t>
   </si>
   <si>
-    <t>+1 movement to leave.</t>
-  </si>
-  <si>
     <t>web.svg</t>
   </si>
   <si>
-    <t>square.svg</t>
-  </si>
-  <si>
     <t>cross1.svg</t>
   </si>
   <si>
@@ -689,12 +600,6 @@
     <t>Pattern</t>
   </si>
   <si>
-    <t>Equip</t>
-  </si>
-  <si>
-    <t>Spawn</t>
-  </si>
-  <si>
     <t>Player 1</t>
   </si>
   <si>
@@ -779,15 +684,9 @@
     <t>[ap]: Move to the opposite side of an adjacent player, creature, or obstacle.</t>
   </si>
   <si>
-    <t>[ap]: Reveal the next three enemy action cards</t>
-  </si>
-  <si>
     <t>[ap]: Remove an adjacent trap. Gain 1 [ar].</t>
   </si>
   <si>
-    <t>[ap]: Target adjacent creature is grabbed.</t>
-  </si>
-  <si>
     <t>[ap]: Move an adjacent obstacle one space in any direction.</t>
   </si>
   <si>
@@ -803,18 +702,6 @@
     <t>Serendipity</t>
   </si>
   <si>
-    <t>Place any ground tile on the bottom of the deck and replace it with the next one in the deck.</t>
-  </si>
-  <si>
-    <t>If your top card is [agl], deal 2 damage to target.</t>
-  </si>
-  <si>
-    <t>Deal 1 damage to creature. If the attack hits, inflict [agl] Fire.</t>
-  </si>
-  <si>
-    <t>Deal 1 damage to creature. If the attack hits, inflict [agl] Confusion.</t>
-  </si>
-  <si>
     <t>north.svg</t>
   </si>
   <si>
@@ -846,6 +733,168 @@
   </si>
   <si>
     <t>shield.svg</t>
+  </si>
+  <si>
+    <t>[ap]: Reveal the next 2 enemy action cards</t>
+  </si>
+  <si>
+    <t>Place any ground tile on the bottom of the deck and replace it with the next one.</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Heal 2 any player.</t>
+  </si>
+  <si>
+    <t>Heal 1 + [int] any player.</t>
+  </si>
+  <si>
+    <t>Deal [agl] damage.</t>
+  </si>
+  <si>
+    <t>Deal 2 + [str] damage.</t>
+  </si>
+  <si>
+    <t>Deal 4 + [str] damage.</t>
+  </si>
+  <si>
+    <t>Deal [int] damage.</t>
+  </si>
+  <si>
+    <t>[ap]: Target adjacent creature is grabbed. If it moves you move in the same direction.</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Reduce damage by [str].</t>
+  </si>
+  <si>
+    <t>Coin</t>
+  </si>
+  <si>
+    <t>coin.svg</t>
+  </si>
+  <si>
+    <t>Costs +1 movement to leave.</t>
+  </si>
+  <si>
+    <t>Deal 3 + [str] damage to all enemies in range.</t>
+  </si>
+  <si>
+    <t>Draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Glass Cannon</t>
+  </si>
+  <si>
+    <t>Fluke</t>
+  </si>
+  <si>
+    <t>Chance</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>chance.svg</t>
+  </si>
+  <si>
+    <t>star.svg</t>
+  </si>
+  <si>
+    <t>Heal for 4.</t>
+  </si>
+  <si>
+    <t>Warp</t>
+  </si>
+  <si>
+    <t>Can't be poisoned.</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>Heal for 5.</t>
+  </si>
+  <si>
+    <t>Flame Guy</t>
+  </si>
+  <si>
+    <t>MagicRange</t>
+  </si>
+  <si>
+    <t>RangedRange</t>
+  </si>
+  <si>
+    <t>MeleeRange</t>
+  </si>
+  <si>
+    <t>diag2.svg</t>
+  </si>
+  <si>
+    <t>Takes 1 damage if it enters water. +3 damage from water attacks.</t>
+  </si>
+  <si>
+    <t>Star / Chance</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Kabura-ya</t>
+  </si>
+  <si>
+    <t>5 damage.</t>
+  </si>
+  <si>
+    <t>9 damage.</t>
+  </si>
+  <si>
+    <t>7 damage.</t>
+  </si>
+  <si>
+    <t>2 Fire damage.</t>
+  </si>
+  <si>
+    <t>11 damage.</t>
+  </si>
+  <si>
+    <t>3 damage and 1 Poison.</t>
+  </si>
+  <si>
+    <t>Deal 6 damage and inflict [int] Fire.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage and inflict [int] Fire.</t>
+  </si>
+  <si>
+    <t>Deal 6 damage and inflict [int] Ice.</t>
+  </si>
+  <si>
+    <t>Deal 1 damage and inflict [agl] Confusion.</t>
+  </si>
+  <si>
+    <t>Deal 1 damage and inflict [agl] Fire.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deal 5 damage and inflict [int] poison. </t>
+  </si>
+  <si>
+    <t>Deal 1 damage and inflict [agl] poison.</t>
+  </si>
+  <si>
+    <t>Snake Dude</t>
+  </si>
+  <si>
+    <t>Bobicorn</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>Deal 1 + [agl] damage.</t>
   </si>
 </sst>
 </file>
@@ -904,7 +953,103 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1279,11 +1424,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1295,9 +1440,9 @@
     <col min="7" max="7" width="105.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="13.2">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1306,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -1318,9 +1463,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="13.2">
       <c r="A2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1329,7 +1474,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E2" s="2">
         <v>4</v>
@@ -1339,9 +1484,9 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="13.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -1350,21 +1495,21 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E3" s="2">
         <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="13.2">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -1373,21 +1518,21 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E4" s="2">
         <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="13.2">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -1396,7 +1541,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E5" s="2">
         <v>4</v>
@@ -1405,10 +1550,10 @@
         <v>8</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="13.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1419,7 +1564,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E6" s="2">
         <v>3</v>
@@ -1429,7 +1574,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="13.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1440,7 +1585,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E7" s="2">
         <v>3</v>
@@ -1452,9 +1597,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="13.2">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
@@ -1463,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E8" s="2">
         <v>3</v>
@@ -1475,9 +1620,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="13.2">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
@@ -1486,21 +1631,21 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E9" s="2">
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="13.2">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
@@ -1509,7 +1654,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E10" s="2">
         <v>3</v>
@@ -1521,7 +1666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="13.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1532,19 +1677,19 @@
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E11" s="2">
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="13.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1555,19 +1700,19 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E12" s="2">
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="13.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1578,7 +1723,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E13" s="2">
         <v>3</v>
@@ -1590,7 +1735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="13.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1601,7 +1746,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E14" s="2">
         <v>3</v>
@@ -1613,7 +1758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="13.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1624,7 +1769,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E15" s="2">
         <v>3</v>
@@ -1636,7 +1781,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" ht="13.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1647,7 +1792,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E16" s="2">
         <v>3</v>
@@ -1659,7 +1804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="13.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1670,7 +1815,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E17" s="2">
         <v>3</v>
@@ -1682,9 +1827,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="13.2">
       <c r="A18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" s="2">
         <v>2</v>
@@ -1693,7 +1838,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="E18" s="2">
         <v>3</v>
@@ -1705,9 +1850,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="13.2">
       <c r="A19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -1716,7 +1861,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E19" s="2">
         <v>3</v>
@@ -1726,7 +1871,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" ht="13.2">
       <c r="A20">
         <v>4</v>
       </c>
@@ -1737,7 +1882,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E20" s="2">
         <v>2</v>
@@ -1747,7 +1892,7 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="13.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1758,7 +1903,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E21" s="2">
         <v>2</v>
@@ -1770,7 +1915,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="13.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1781,7 +1926,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E22" s="2">
         <v>2</v>
@@ -1793,7 +1938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="13.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1804,7 +1949,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E23" s="2">
         <v>2</v>
@@ -1816,7 +1961,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="13.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1827,19 +1972,19 @@
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E24" s="2">
         <v>2</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="13.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1850,7 +1995,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
@@ -1859,33 +2004,33 @@
         <v>40</v>
       </c>
       <c r="G25" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="13.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="13.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1896,7 +2041,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
@@ -1908,7 +2053,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" ht="13.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1919,7 +2064,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E28" s="2">
         <v>2</v>
@@ -1931,7 +2076,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" ht="13.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1942,7 +2087,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E29" s="2">
         <v>2</v>
@@ -1954,7 +2099,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="13.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1965,7 +2110,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E30" s="2">
         <v>2</v>
@@ -1974,10 +2119,10 @@
         <v>47</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="13.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1988,7 +2133,7 @@
         <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E31" s="2">
         <v>2</v>
@@ -2000,7 +2145,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" ht="13.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -2011,7 +2156,7 @@
         <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E32" s="2">
         <v>2</v>
@@ -2023,7 +2168,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" ht="13.2">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2034,7 +2179,7 @@
         <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E33" s="2">
         <v>2</v>
@@ -2046,9 +2191,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" ht="13.2">
       <c r="A34">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
@@ -2057,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="E34" s="2">
         <v>4</v>
@@ -2067,7 +2212,7 @@
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" ht="13.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2078,7 +2223,7 @@
         <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="E35" s="2">
         <v>1</v>
@@ -2088,7 +2233,7 @@
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" ht="13.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2099,7 +2244,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="E36" s="2">
         <v>1</v>
@@ -2108,12 +2253,12 @@
         <v>56</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="13.2">
       <c r="A37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" s="2">
         <v>2</v>
@@ -2122,7 +2267,7 @@
         <v>3</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="E37" s="2">
         <v>1</v>
@@ -2131,306 +2276,309 @@
         <v>57</v>
       </c>
       <c r="G37" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="13.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="2">
-        <v>2</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:7" ht="13.2">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2</v>
+      </c>
+      <c r="C39" s="2">
+        <v>3</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" s="2">
-        <v>2</v>
-      </c>
-      <c r="C39" s="2">
-        <v>3</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E39" s="2">
-        <v>1</v>
-      </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="13.2">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="13.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="13.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E42" s="2">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" s="2">
-        <v>1</v>
-      </c>
-      <c r="C40" s="2">
-        <v>2</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E40" s="2">
-        <v>1</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="B41" s="2">
-        <v>1</v>
-      </c>
-      <c r="C41" s="2">
-        <v>2</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E41" s="2">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" s="1">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2">
-        <v>2</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E42" s="2">
-        <v>1</v>
-      </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G42" s="2" t="s">
+    </row>
+    <row r="43" spans="1:7" ht="13.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43" s="1">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2">
-        <v>2</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E43" s="2">
-        <v>1</v>
-      </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:7" ht="13.2">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-      <c r="C44" s="2">
-        <v>2</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E44" s="2">
-        <v>1</v>
-      </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="13.2">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2</v>
+      </c>
+      <c r="C45" s="2">
+        <v>3</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" s="2">
-        <v>2</v>
-      </c>
-      <c r="C45" s="2">
-        <v>3</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E45" s="2">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2" t="s">
+    <row r="46" spans="1:7" ht="13.2">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" s="2">
-        <v>1</v>
-      </c>
-      <c r="C46" s="2">
-        <v>2</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E46" s="2">
-        <v>1</v>
-      </c>
-      <c r="F46" s="2" t="s">
+    <row r="47" spans="1:7" ht="13.2">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" s="2">
-        <v>2</v>
-      </c>
-      <c r="C47" s="2">
-        <v>3</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E47" s="2">
-        <v>1</v>
-      </c>
-      <c r="F47" s="2" t="s">
+    <row r="48" spans="1:7" ht="13.2">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" s="2">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2">
+        <v>3</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48" s="2">
-        <v>2</v>
-      </c>
-      <c r="C48" s="2">
-        <v>3</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E48" s="2">
-        <v>1</v>
-      </c>
-      <c r="F48" s="2" t="s">
+    <row r="49" spans="1:7" ht="13.2">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" s="2">
+        <v>2</v>
+      </c>
+      <c r="C49" s="2">
+        <v>3</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="B49" s="2">
-        <v>2</v>
-      </c>
-      <c r="C49" s="2">
-        <v>3</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E49" s="2">
-        <v>2</v>
-      </c>
-      <c r="F49" s="2" t="s">
+    <row r="50" spans="1:7" ht="13.2">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" s="2">
+        <v>2</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="B50" s="2">
-        <v>2</v>
-      </c>
-      <c r="C50" s="2">
-        <v>2</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E50" s="2">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" ht="13.2">
       <c r="A51">
         <v>2</v>
       </c>
@@ -2441,41 +2589,41 @@
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="E51" s="2">
         <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="13.2">
       <c r="A52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B52" s="2">
         <v>2</v>
       </c>
       <c r="C52" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="E52" s="2">
         <v>3</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1">
       <c r="A53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B53" s="2">
         <v>2</v>
@@ -2484,140 +2632,240 @@
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="E53" s="2">
         <v>0</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1">
       <c r="A54">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B54" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C54" s="2">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="E54" s="2">
         <v>0</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>83</v>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" s="2">
+        <v>2</v>
+      </c>
+      <c r="C55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E55" s="2">
+        <v>4</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="13.2">
+      <c r="A56">
+        <v>8</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0</v>
+      </c>
+      <c r="C56" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D8 D54:D1041 D10:D39 D42:D52">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="str">
+  <conditionalFormatting sqref="D1:D8 D10:D39 D42:D53 D56:D1041">
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="str">
       <formula>NOT(ISERROR(SEARCH(("str"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D8 D54:D1041 D10:D39 D42:D52">
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="agl">
+  <conditionalFormatting sqref="D1:D8 D10:D39 D42:D53 D56:D1041">
+    <cfRule type="containsText" dxfId="30" priority="34" operator="containsText" text="agl">
       <formula>NOT(ISERROR(SEARCH(("agl"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D8 D54:D1041 D10:D39 D42:D52">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="int">
+  <conditionalFormatting sqref="D1:D8 D10:D39 D42:D53 D56:D1041">
+    <cfRule type="containsText" dxfId="29" priority="35" operator="containsText" text="int">
       <formula>NOT(ISERROR(SEARCH(("int"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D8 D54:D1041 D10:D39 D42:D52">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="any">
+  <conditionalFormatting sqref="D1:D8 D10:D39 D42:D53 D56:D1041">
+    <cfRule type="containsText" dxfId="28" priority="36" operator="containsText" text="any">
       <formula>NOT(ISERROR(SEARCH(("any"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D54">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="str">
-      <formula>NOT(ISERROR(SEARCH(("str"),(D53))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D54">
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="agl">
-      <formula>NOT(ISERROR(SEARCH(("agl"),(D53))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D54">
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="int">
-      <formula>NOT(ISERROR(SEARCH(("int"),(D53))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D54">
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="any">
-      <formula>NOT(ISERROR(SEARCH(("any"),(D53))))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="str">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="str">
       <formula>NOT(ISERROR(SEARCH(("str"),(D9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="agl">
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="agl">
       <formula>NOT(ISERROR(SEARCH(("agl"),(D9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="int">
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="int">
       <formula>NOT(ISERROR(SEARCH(("int"),(D9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="any">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="any">
       <formula>NOT(ISERROR(SEARCH(("any"),(D9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="str">
+    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="str">
       <formula>NOT(ISERROR(SEARCH(("str"),(D40))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="agl">
+    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="agl">
       <formula>NOT(ISERROR(SEARCH(("agl"),(D40))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="int">
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="int">
       <formula>NOT(ISERROR(SEARCH(("int"),(D40))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="any">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="any">
       <formula>NOT(ISERROR(SEARCH(("any"),(D40))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="str">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="str">
       <formula>NOT(ISERROR(SEARCH(("str"),(D41))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="agl">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="agl">
       <formula>NOT(ISERROR(SEARCH(("agl"),(D41))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="int">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="int">
       <formula>NOT(ISERROR(SEARCH(("int"),(D41))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="any">
+      <formula>NOT(ISERROR(SEARCH(("any"),(D41))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="str">
+      <formula>NOT(ISERROR(SEARCH(("str"),(D54))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="agl">
+      <formula>NOT(ISERROR(SEARCH(("agl"),(D54))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="int">
+      <formula>NOT(ISERROR(SEARCH(("int"),(D54))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="any">
+      <formula>NOT(ISERROR(SEARCH(("any"),(D54))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="str">
+      <formula>NOT(ISERROR(SEARCH(("str"),(D54))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="agl">
+      <formula>NOT(ISERROR(SEARCH(("agl"),(D54))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="int">
+      <formula>NOT(ISERROR(SEARCH(("int"),(D54))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="any">
+      <formula>NOT(ISERROR(SEARCH(("any"),(D54))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55:D56">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="str">
+      <formula>NOT(ISERROR(SEARCH(("str"),(D55))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55:D56">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="agl">
+      <formula>NOT(ISERROR(SEARCH(("agl"),(D55))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55:D56">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="int">
+      <formula>NOT(ISERROR(SEARCH(("int"),(D55))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55:D56">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="any">
+      <formula>NOT(ISERROR(SEARCH(("any"),(D55))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55:D56">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="str">
+      <formula>NOT(ISERROR(SEARCH(("str"),(D55))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55:D56">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="agl">
+      <formula>NOT(ISERROR(SEARCH(("agl"),(D55))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55:D56">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="int">
+      <formula>NOT(ISERROR(SEARCH(("int"),(D55))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55:D56">
     <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="any">
-      <formula>NOT(ISERROR(SEARCH(("any"),(D41))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("any"),(D55))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2633,7 +2881,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2642,18 +2890,18 @@
     <col min="6" max="6" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="13.2">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -2662,10 +2910,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2674,163 +2922,166 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="13.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="13.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="G5" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="13.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="G6" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="G8" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="13.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="13.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="13.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>100</v>
+      <c r="F11" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
@@ -2838,13 +3089,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
@@ -2852,13 +3103,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
@@ -2866,13 +3117,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
@@ -2880,13 +3131,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
@@ -2894,13 +3145,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="3:3" ht="15.75" customHeight="1">
@@ -2945,9 +3196,9 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2959,94 +3210,94 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>248</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3079,279 +3330,363 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="6" max="6" width="99.44140625" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" customWidth="1"/>
+    <col min="7" max="7" width="99.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>217</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>103</v>
+        <v>267</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>216</v>
+        <v>100</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="F8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>183</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>137</v>
+        <v>122</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>138</v>
+        <v>225</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>214</v>
+        <v>123</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>183</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>137</v>
+        <v>124</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>142</v>
+        <v>227</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>214</v>
+        <v>125</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>184</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>137</v>
+        <v>126</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>145</v>
+        <v>227</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>214</v>
+        <v>127</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>184</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>148</v>
+        <v>227</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>214</v>
+        <v>129</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>149</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3363,11 +3698,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3379,19 +3714,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="D1" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="E1" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3399,10 +3734,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3410,13 +3745,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="D3" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3424,10 +3759,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3435,13 +3770,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="D5" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3449,10 +3784,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3460,13 +3795,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="D7" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3474,10 +3809,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3485,13 +3820,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="D9" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3499,10 +3834,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3510,13 +3845,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="D11" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3524,10 +3859,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3535,13 +3870,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="C13" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="D13" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3549,10 +3884,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3560,13 +3895,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="C15" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="D15" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3574,13 +3909,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="E16" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3588,13 +3923,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="E17" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3602,13 +3937,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="E18" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3616,16 +3951,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="D19" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="E19" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3633,16 +3968,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="D20" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="E20" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3650,16 +3985,52 @@
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="D21" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="E21" t="s">
-        <v>269</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D24" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3672,11 +4043,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3684,6 +4055,9 @@
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="4" width="5" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
+    <col min="10" max="10" width="20.21875" customWidth="1"/>
     <col min="13" max="13" width="57" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3695,45 +4069,45 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>160</v>
+        <v>283</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -3745,28 +4119,184 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>125</v>
+        <v>181</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>161</v>
+        <v>271</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>162</v>
+        <v>269</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>139</v>
+        <v>184</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>163</v>
+        <v>274</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1761442E-A2FD-436B-90B8-D060C3878F32}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>164</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>165</v>
+      <c r="B1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>